<commit_message>
change google to MS
</commit_message>
<xml_diff>
--- a/generateEXCEL/Data/Members/GroupRecord.xlsx
+++ b/generateEXCEL/Data/Members/GroupRecord.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hguan/Dropbox/Research/Coding/WeChatGroup/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hguan/GitHub/lc-score-board/generateEXCEL/Data/Members/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE229AD5-DC99-A243-A525-37E2F95C0359}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ADE789C-5855-AC40-BC79-E95CF6140AF3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-41860" yWindow="1980" windowWidth="19000" windowHeight="14340" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-41860" yWindow="1980" windowWidth="19000" windowHeight="14340" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Current" sheetId="1" r:id="rId1"/>
@@ -5318,8 +5318,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K243"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A116" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B123" sqref="B123"/>
+    <sheetView topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -5832,7 +5832,7 @@
         <v>91</v>
       </c>
       <c r="G24" s="4" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="H24" s="7"/>
       <c r="J24" s="8" t="s">
@@ -7394,7 +7394,7 @@
         <v>151</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="J102" s="8" t="s">
         <v>412</v>
@@ -8376,8 +8376,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L414"/>
   <sheetViews>
-    <sheetView topLeftCell="A390" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D414" sqref="D414"/>
+    <sheetView tabSelected="1" topLeftCell="B302" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G319" sqref="G319"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.6640625" defaultRowHeight="15"/>
@@ -16483,7 +16483,7 @@
         <v>89</v>
       </c>
       <c r="G318" s="33" t="s">
-        <v>1</v>
+        <v>45</v>
       </c>
       <c r="H318" s="33"/>
       <c r="J318" s="45" t="s">

</xml_diff>